<commit_message>
Sofia | Waight of frame | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Strength/SSS_Sofia_Strength.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Strength/SSS_Sofia_Strength.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E8C0B0-BB08-4866-A663-CE0DF2FF182E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F70CE-BF7B-4BFE-A23F-CA648AB15507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StrengthLimSea" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <r>
       <t>Bending moment min [kN</t>
@@ -79,12 +79,6 @@
     <t>Waight [t]</t>
   </si>
   <si>
-    <t>Fr.min</t>
-  </si>
-  <si>
-    <t>Fr.max</t>
-  </si>
-  <si>
     <t>The value of conditional displacement [m3]</t>
   </si>
   <si>
@@ -98,6 +92,15 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Fr,min</t>
+  </si>
+  <si>
+    <t>Fr,max</t>
   </si>
 </sst>
 </file>
@@ -215,11 +218,11 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -807,10 +810,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E38C0ED-6F7D-4E89-BD94-0E5CB0E212B1}">
-  <dimension ref="A1:C140"/>
+  <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,18 +823,18 @@
     <col min="4" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>-5.3333333333333304</v>
       </c>
@@ -842,7 +845,7 @@
         <v>0.48667369595736798</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>-5</v>
       </c>
@@ -853,7 +856,7 @@
         <v>2.6648656987425401</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>-4.6666666666666696</v>
       </c>
@@ -864,7 +867,7 @@
         <v>4.37856457639821</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>-4</v>
       </c>
@@ -875,7 +878,7 @@
         <v>11.903173361029999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>-3</v>
       </c>
@@ -885,8 +888,11 @@
       <c r="C6" s="7">
         <v>13.695603273876401</v>
       </c>
+      <c r="G6" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>-2</v>
       </c>
@@ -897,7 +903,7 @@
         <v>36.814951775159798</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>0</v>
       </c>
@@ -908,7 +914,7 @@
         <v>14.9892700805395</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -919,7 +925,7 @@
         <v>9.2600885831904591</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>1.6666666666666701</v>
       </c>
@@ -930,7 +936,7 @@
         <v>12.505295929021599</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>2.5</v>
       </c>
@@ -941,7 +947,7 @@
         <v>7.7052005944126902</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -952,7 +958,7 @@
         <v>5.2606918729713197</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>3.3333333333333299</v>
       </c>
@@ -963,7 +969,7 @@
         <v>9.1225090965689706</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>3.8333333333333299</v>
       </c>
@@ -974,7 +980,7 @@
         <v>24.370152853508799</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>5</v>
       </c>
@@ -985,7 +991,7 @@
         <v>18.390890415699602</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>5.8333333333333304</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>114</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C67" s="5">
         <v>155.99373657530001</v>
@@ -1559,7 +1565,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B68" s="7">
         <v>119</v>
@@ -1797,567 +1803,6 @@
       </c>
       <c r="C89" s="7">
         <v>5.3752914889180402E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="7">
-        <v>83</v>
-      </c>
-      <c r="B90" s="7">
-        <v>84</v>
-      </c>
-      <c r="C90" s="7">
-        <v>12.2605516458975</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="7">
-        <v>84</v>
-      </c>
-      <c r="B91" s="7">
-        <v>85</v>
-      </c>
-      <c r="C91" s="7">
-        <v>12.1686071027198</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="5">
-        <v>85</v>
-      </c>
-      <c r="B92" s="5">
-        <v>86</v>
-      </c>
-      <c r="C92" s="5">
-        <v>12.0766625595418</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="7">
-        <v>86</v>
-      </c>
-      <c r="B93" s="7">
-        <v>87</v>
-      </c>
-      <c r="C93" s="7">
-        <v>11.984718016364001</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="7">
-        <v>87</v>
-      </c>
-      <c r="B94" s="7">
-        <v>88</v>
-      </c>
-      <c r="C94" s="7">
-        <v>11.8759198474761</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="7">
-        <v>88</v>
-      </c>
-      <c r="B95" s="7">
-        <v>89</v>
-      </c>
-      <c r="C95" s="7">
-        <v>11.7111853171207</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="7">
-        <v>89</v>
-      </c>
-      <c r="B96" s="7">
-        <v>90</v>
-      </c>
-      <c r="C96" s="7">
-        <v>11.5073680510079</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="5">
-        <v>90</v>
-      </c>
-      <c r="B97" s="5">
-        <v>91</v>
-      </c>
-      <c r="C97" s="5">
-        <v>11.303550784894901</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="7">
-        <v>91</v>
-      </c>
-      <c r="B98" s="7">
-        <v>92</v>
-      </c>
-      <c r="C98" s="7">
-        <v>11.0997335187822</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="7">
-        <v>92</v>
-      </c>
-      <c r="B99" s="7">
-        <v>93</v>
-      </c>
-      <c r="C99" s="7">
-        <v>10.895916252669201</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="7">
-        <v>93</v>
-      </c>
-      <c r="B100" s="7">
-        <v>94</v>
-      </c>
-      <c r="C100" s="7">
-        <v>10.6920989865566</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="7">
-        <v>94</v>
-      </c>
-      <c r="B101" s="7">
-        <v>95</v>
-      </c>
-      <c r="C101" s="7">
-        <v>10.488281720443601</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="5">
-        <v>95</v>
-      </c>
-      <c r="B102" s="5">
-        <v>96</v>
-      </c>
-      <c r="C102" s="5">
-        <v>10.2089711086803</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="7">
-        <v>96</v>
-      </c>
-      <c r="B103" s="7">
-        <v>97</v>
-      </c>
-      <c r="C103" s="7">
-        <v>9.8422738252527306</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="7">
-        <v>97</v>
-      </c>
-      <c r="B104" s="7">
-        <v>98</v>
-      </c>
-      <c r="C104" s="7">
-        <v>9.4636832158123507</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="7">
-        <v>98</v>
-      </c>
-      <c r="B105" s="7">
-        <v>99</v>
-      </c>
-      <c r="C105" s="7">
-        <v>9.0850926063715196</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="7">
-        <v>99</v>
-      </c>
-      <c r="B106" s="7">
-        <v>100</v>
-      </c>
-      <c r="C106" s="7">
-        <v>8.7065019969306796</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="5">
-        <v>100</v>
-      </c>
-      <c r="B107" s="5">
-        <v>101</v>
-      </c>
-      <c r="C107" s="5">
-        <v>7.1413773150520701</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="7">
-        <v>101</v>
-      </c>
-      <c r="B108" s="7">
-        <v>102</v>
-      </c>
-      <c r="C108" s="7">
-        <v>6.8224803827404203</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="7">
-        <v>102</v>
-      </c>
-      <c r="B109" s="7">
-        <v>103</v>
-      </c>
-      <c r="C109" s="7">
-        <v>6.5095086899561903</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="7">
-        <v>103</v>
-      </c>
-      <c r="B110" s="7">
-        <v>104</v>
-      </c>
-      <c r="C110" s="7">
-        <v>6.2197113660549803</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="7">
-        <v>104</v>
-      </c>
-      <c r="B111" s="7">
-        <v>105</v>
-      </c>
-      <c r="C111" s="7">
-        <v>5.9464373671671602</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="5">
-        <v>105</v>
-      </c>
-      <c r="B112" s="5">
-        <v>106</v>
-      </c>
-      <c r="C112" s="5">
-        <v>5.7023562866102102</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="7">
-        <v>106</v>
-      </c>
-      <c r="B113" s="7">
-        <v>107</v>
-      </c>
-      <c r="C113" s="7">
-        <v>5.5044665325265196</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="7">
-        <v>107</v>
-      </c>
-      <c r="B114" s="7">
-        <v>108</v>
-      </c>
-      <c r="C114" s="7">
-        <v>5.3235751865845504</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="7">
-        <v>108</v>
-      </c>
-      <c r="B115" s="7">
-        <v>109</v>
-      </c>
-      <c r="C115" s="7">
-        <v>5.1426838406427997</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="7">
-        <v>109</v>
-      </c>
-      <c r="B116" s="7">
-        <v>110</v>
-      </c>
-      <c r="C116" s="7">
-        <v>4.9617924947012897</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="5">
-        <v>110</v>
-      </c>
-      <c r="B117" s="5">
-        <v>111</v>
-      </c>
-      <c r="C117" s="5">
-        <v>4.7809011487595399</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="7">
-        <v>111</v>
-      </c>
-      <c r="B118" s="7">
-        <v>112</v>
-      </c>
-      <c r="C118" s="7">
-        <v>4.60000980281779</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="7">
-        <v>112</v>
-      </c>
-      <c r="B119" s="7">
-        <v>113</v>
-      </c>
-      <c r="C119" s="7">
-        <v>4.41911845687605</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="7">
-        <v>113</v>
-      </c>
-      <c r="B120" s="7">
-        <v>114</v>
-      </c>
-      <c r="C120" s="7">
-        <v>5.5028282293305901</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="7">
-        <v>114</v>
-      </c>
-      <c r="B121" s="7">
-        <v>115</v>
-      </c>
-      <c r="C121" s="7">
-        <v>6.52032407845513</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="5">
-        <v>115</v>
-      </c>
-      <c r="B122" s="5">
-        <v>116</v>
-      </c>
-      <c r="C122" s="5">
-        <v>6.2070048858529399</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="7">
-        <v>116</v>
-      </c>
-      <c r="B123" s="7">
-        <v>117</v>
-      </c>
-      <c r="C123" s="7">
-        <v>5.8936178803030499</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="7">
-        <v>117</v>
-      </c>
-      <c r="B124" s="7">
-        <v>118</v>
-      </c>
-      <c r="C124" s="7">
-        <v>5.5705433107386897</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="7">
-        <v>118</v>
-      </c>
-      <c r="B125" s="7">
-        <v>119</v>
-      </c>
-      <c r="C125" s="7">
-        <v>5.2378489901086596</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="7">
-        <v>119</v>
-      </c>
-      <c r="B126" s="7">
-        <v>120</v>
-      </c>
-      <c r="C126" s="7">
-        <v>4.9051546694786303</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="5">
-        <v>120</v>
-      </c>
-      <c r="B127" s="5">
-        <v>121</v>
-      </c>
-      <c r="C127" s="5">
-        <v>4.5773896599623596</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="7">
-        <v>121</v>
-      </c>
-      <c r="B128" s="7">
-        <v>122</v>
-      </c>
-      <c r="C128" s="7">
-        <v>4.2547540064442702</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="7">
-        <v>122</v>
-      </c>
-      <c r="B129" s="7">
-        <v>123</v>
-      </c>
-      <c r="C129" s="7">
-        <v>3.9323183978099201</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="7">
-        <v>123</v>
-      </c>
-      <c r="B130" s="7">
-        <v>124</v>
-      </c>
-      <c r="C130" s="7">
-        <v>3.6019090675893</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="7">
-        <v>124</v>
-      </c>
-      <c r="B131" s="7">
-        <v>125</v>
-      </c>
-      <c r="C131" s="7">
-        <v>3.2617399802247702</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="5">
-        <v>125</v>
-      </c>
-      <c r="B132" s="5">
-        <v>126</v>
-      </c>
-      <c r="C132" s="5">
-        <v>2.9170215317994899</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="7">
-        <v>126</v>
-      </c>
-      <c r="B133" s="7">
-        <v>127</v>
-      </c>
-      <c r="C133" s="7">
-        <v>2.5304345151421299</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="7">
-        <v>127</v>
-      </c>
-      <c r="B134" s="7">
-        <v>128</v>
-      </c>
-      <c r="C134" s="7">
-        <v>2.1071723997395102</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="7">
-        <v>128</v>
-      </c>
-      <c r="B135" s="7">
-        <v>129</v>
-      </c>
-      <c r="C135" s="7">
-        <v>1.6960610042556299</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="7">
-        <v>129</v>
-      </c>
-      <c r="B136" s="7">
-        <v>130</v>
-      </c>
-      <c r="C136" s="7">
-        <v>1.2820462725819699</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="5">
-        <v>130</v>
-      </c>
-      <c r="B137" s="5">
-        <v>131</v>
-      </c>
-      <c r="C137" s="5">
-        <v>0.55243373779262595</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="7">
-        <v>131</v>
-      </c>
-      <c r="B138" s="7">
-        <v>132</v>
-      </c>
-      <c r="C138" s="7">
-        <v>1.8070262451146801E-2</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="7">
-        <v>132</v>
-      </c>
-      <c r="B139" s="7">
-        <v>133</v>
-      </c>
-      <c r="C139" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="7">
-        <v>133</v>
-      </c>
-      <c r="B140" s="7">
-        <v>134</v>
-      </c>
-      <c r="C140" s="7">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2370,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20BEA4F-BC0F-43C3-9757-F9D5D695856A}">
   <dimension ref="A1:DQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2382,84 +1827,84 @@
   <sheetData>
     <row r="1" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="13">
+        <v>9</v>
+      </c>
+      <c r="B1" s="12">
         <f>130.5/60</f>
         <v>2.1749999999999998</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="13"/>
-      <c r="BO1" s="13"/>
-      <c r="BP1" s="13"/>
-      <c r="BQ1" s="13"/>
-      <c r="BR1" s="13"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
+      <c r="BB1" s="12"/>
+      <c r="BC1" s="12"/>
+      <c r="BD1" s="12"/>
+      <c r="BE1" s="12"/>
+      <c r="BF1" s="12"/>
+      <c r="BG1" s="12"/>
+      <c r="BH1" s="12"/>
+      <c r="BI1" s="12"/>
+      <c r="BJ1" s="12"/>
+      <c r="BK1" s="12"/>
+      <c r="BL1" s="12"/>
+      <c r="BM1" s="12"/>
+      <c r="BN1" s="12"/>
+      <c r="BO1" s="12"/>
+      <c r="BP1" s="12"/>
+      <c r="BQ1" s="12"/>
+      <c r="BR1" s="12"/>
     </row>
     <row r="2" spans="1:121" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="9">
         <v>0.1</v>
@@ -2824,130 +2269,130 @@
     </row>
     <row r="3" spans="1:121" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="12"/>
-      <c r="AV3" s="12"/>
-      <c r="AW3" s="12"/>
-      <c r="AX3" s="12"/>
-      <c r="AY3" s="12"/>
-      <c r="AZ3" s="12"/>
-      <c r="BA3" s="12"/>
-      <c r="BB3" s="12"/>
-      <c r="BC3" s="12"/>
-      <c r="BD3" s="12"/>
-      <c r="BE3" s="12"/>
-      <c r="BF3" s="12"/>
-      <c r="BG3" s="12"/>
-      <c r="BH3" s="12"/>
-      <c r="BI3" s="12"/>
-      <c r="BJ3" s="12"/>
-      <c r="BK3" s="12"/>
-      <c r="BL3" s="12"/>
-      <c r="BM3" s="12"/>
-      <c r="BN3" s="12"/>
-      <c r="BO3" s="12"/>
-      <c r="BP3" s="12"/>
-      <c r="BQ3" s="12"/>
-      <c r="BR3" s="12"/>
-      <c r="BS3" s="12"/>
-      <c r="BT3" s="12"/>
-      <c r="BU3" s="12"/>
-      <c r="BV3" s="12"/>
-      <c r="BW3" s="12"/>
-      <c r="BX3" s="12"/>
-      <c r="BY3" s="12"/>
-      <c r="BZ3" s="12"/>
-      <c r="CA3" s="12"/>
-      <c r="CB3" s="12"/>
-      <c r="CC3" s="12"/>
-      <c r="CD3" s="12"/>
-      <c r="CE3" s="12"/>
-      <c r="CF3" s="12"/>
-      <c r="CG3" s="12"/>
-      <c r="CH3" s="12"/>
-      <c r="CI3" s="12"/>
-      <c r="CJ3" s="12"/>
-      <c r="CK3" s="12"/>
-      <c r="CL3" s="12"/>
-      <c r="CM3" s="12"/>
-      <c r="CN3" s="12"/>
-      <c r="CO3" s="12"/>
-      <c r="CP3" s="12"/>
-      <c r="CQ3" s="12"/>
-      <c r="CR3" s="12"/>
-      <c r="CS3" s="12"/>
-      <c r="CT3" s="12"/>
-      <c r="CU3" s="12"/>
-      <c r="CV3" s="12"/>
-      <c r="CW3" s="12"/>
-      <c r="CX3" s="12"/>
-      <c r="CY3" s="12"/>
-      <c r="CZ3" s="12"/>
-      <c r="DA3" s="12"/>
-      <c r="DB3" s="12"/>
-      <c r="DC3" s="12"/>
-      <c r="DD3" s="12"/>
-      <c r="DE3" s="12"/>
-      <c r="DF3" s="12"/>
-      <c r="DG3" s="12"/>
-      <c r="DH3" s="12"/>
-      <c r="DI3" s="12"/>
-      <c r="DJ3" s="12"/>
-      <c r="DK3" s="12"/>
-      <c r="DL3" s="12"/>
-      <c r="DM3" s="12"/>
-      <c r="DN3" s="12"/>
-      <c r="DO3" s="12"/>
-      <c r="DP3" s="12"/>
-      <c r="DQ3" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="13"/>
+      <c r="AV3" s="13"/>
+      <c r="AW3" s="13"/>
+      <c r="AX3" s="13"/>
+      <c r="AY3" s="13"/>
+      <c r="AZ3" s="13"/>
+      <c r="BA3" s="13"/>
+      <c r="BB3" s="13"/>
+      <c r="BC3" s="13"/>
+      <c r="BD3" s="13"/>
+      <c r="BE3" s="13"/>
+      <c r="BF3" s="13"/>
+      <c r="BG3" s="13"/>
+      <c r="BH3" s="13"/>
+      <c r="BI3" s="13"/>
+      <c r="BJ3" s="13"/>
+      <c r="BK3" s="13"/>
+      <c r="BL3" s="13"/>
+      <c r="BM3" s="13"/>
+      <c r="BN3" s="13"/>
+      <c r="BO3" s="13"/>
+      <c r="BP3" s="13"/>
+      <c r="BQ3" s="13"/>
+      <c r="BR3" s="13"/>
+      <c r="BS3" s="13"/>
+      <c r="BT3" s="13"/>
+      <c r="BU3" s="13"/>
+      <c r="BV3" s="13"/>
+      <c r="BW3" s="13"/>
+      <c r="BX3" s="13"/>
+      <c r="BY3" s="13"/>
+      <c r="BZ3" s="13"/>
+      <c r="CA3" s="13"/>
+      <c r="CB3" s="13"/>
+      <c r="CC3" s="13"/>
+      <c r="CD3" s="13"/>
+      <c r="CE3" s="13"/>
+      <c r="CF3" s="13"/>
+      <c r="CG3" s="13"/>
+      <c r="CH3" s="13"/>
+      <c r="CI3" s="13"/>
+      <c r="CJ3" s="13"/>
+      <c r="CK3" s="13"/>
+      <c r="CL3" s="13"/>
+      <c r="CM3" s="13"/>
+      <c r="CN3" s="13"/>
+      <c r="CO3" s="13"/>
+      <c r="CP3" s="13"/>
+      <c r="CQ3" s="13"/>
+      <c r="CR3" s="13"/>
+      <c r="CS3" s="13"/>
+      <c r="CT3" s="13"/>
+      <c r="CU3" s="13"/>
+      <c r="CV3" s="13"/>
+      <c r="CW3" s="13"/>
+      <c r="CX3" s="13"/>
+      <c r="CY3" s="13"/>
+      <c r="CZ3" s="13"/>
+      <c r="DA3" s="13"/>
+      <c r="DB3" s="13"/>
+      <c r="DC3" s="13"/>
+      <c r="DD3" s="13"/>
+      <c r="DE3" s="13"/>
+      <c r="DF3" s="13"/>
+      <c r="DG3" s="13"/>
+      <c r="DH3" s="13"/>
+      <c r="DI3" s="13"/>
+      <c r="DJ3" s="13"/>
+      <c r="DK3" s="13"/>
+      <c r="DL3" s="13"/>
+      <c r="DM3" s="13"/>
+      <c r="DN3" s="13"/>
+      <c r="DO3" s="13"/>
+      <c r="DP3" s="13"/>
+      <c r="DQ3" s="13"/>
     </row>
     <row r="4" spans="1:121" x14ac:dyDescent="0.25">
       <c r="A4" s="9">

</xml_diff>

<commit_message>
Sofia | strengthLim | fix
</commit_message>
<xml_diff>
--- a/assets/fleet/9245263_sofia/datasets/Strength/SSS_Sofia_Strength.xlsx
+++ b/assets/fleet/9245263_sofia/datasets/Strength/SSS_Sofia_Strength.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MERENKOV\Desktop\Капитан\sss\assets\fleet\9245263_sofia\datasets\Strength\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C99D58-AFFF-480D-8654-A687DA476680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298B8D94-63DE-415E-ADFC-F0CC5967EC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StrengthLimSea" sheetId="4" r:id="rId1"/>
@@ -523,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D6ED65C-1F17-45E0-93FA-FEF8356AACAF}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,8 +556,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>28</v>
+      <c r="A2" s="3">
+        <v>-6</v>
       </c>
       <c r="B2" s="2">
         <v>-110507</v>
@@ -574,24 +574,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>-226258</v>
+        <v>-110507</v>
       </c>
       <c r="C3" s="2">
-        <v>250572</v>
+        <v>86516</v>
       </c>
       <c r="D3" s="2">
-        <v>-28400</v>
+        <v>-12418</v>
       </c>
       <c r="E3" s="2">
-        <v>28400</v>
+        <v>12418</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2">
         <v>-226258</v>
@@ -608,25 +608,54 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>117</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-226258</v>
+      </c>
+      <c r="C5" s="2">
+        <v>250572</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-28400</v>
+      </c>
+      <c r="E5" s="2">
+        <v>28400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>156</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
         <v>-37507</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>62855</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>-11000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>180</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-37507</v>
+      </c>
+      <c r="C7" s="2">
+        <v>62855</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-11000</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -636,15 +665,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E4AA85-43BA-4EE3-8CF8-D91FCC00D44D}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -670,7 +699,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>28</v>
+        <v>-6</v>
       </c>
       <c r="B2" s="2">
         <v>-198400</v>
@@ -687,24 +716,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>-314170</v>
+        <v>-198400</v>
       </c>
       <c r="C3" s="2">
-        <v>314170</v>
+        <v>198400</v>
       </c>
       <c r="D3" s="2">
-        <v>-28400</v>
+        <v>-12418</v>
       </c>
       <c r="E3" s="2">
-        <v>28400</v>
+        <v>12418</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2">
         <v>-314170</v>
@@ -721,30 +750,54 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>117</v>
+      </c>
+      <c r="B5" s="2">
+        <v>-314170</v>
+      </c>
+      <c r="C5" s="2">
+        <v>314170</v>
+      </c>
+      <c r="D5" s="2">
+        <v>-28400</v>
+      </c>
+      <c r="E5" s="2">
+        <v>28400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>156</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
         <v>-90000</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="2">
         <v>90000</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="2">
         <v>-11000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E6" s="2">
         <v>11000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-    </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="1">
+        <v>180</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-90000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>90000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>-11000</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11000</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
@@ -784,11 +837,11 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -814,6 +867,11 @@
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -825,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E38C0ED-6F7D-4E89-BD94-0E5CB0E212B1}">
   <dimension ref="A1:G1376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N16" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J174" sqref="J174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>